<commit_message>
Full template, sans qualitative
</commit_message>
<xml_diff>
--- a/output/drc/publisher.xlsx
+++ b/output/drc/publisher.xlsx
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A166" activeCellId="0" sqref="A166"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A153" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A193" activeCellId="0" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="B158" s="64" t="inlineStr">
         <is>
-          <t>7, 10, 5, 8, 4, 1, 3, 9, 6, 2</t>
+          <t>5, 3, 10, 6, 8, 9, 1, 7, 4, 2</t>
         </is>
       </c>
     </row>
@@ -2692,7 +2692,9 @@
           <t>Activity level: Number of activities including default finance type</t>
         </is>
       </c>
-      <c r="B171" s="71" t="n"/>
+      <c r="B171" s="71" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="172" ht="13.8" customHeight="1" s="45">
       <c r="A172" s="73" t="inlineStr">
@@ -2700,7 +2702,9 @@
           <t>Activity level: Percentage of activities including default finance type</t>
         </is>
       </c>
-      <c r="B172" s="72" t="n"/>
+      <c r="B172" s="72" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="173" ht="13.8" customHeight="1" s="45">
       <c r="A173" s="73" t="inlineStr">
@@ -2708,7 +2712,9 @@
           <t>Transaction level: Number of transactions including finance type</t>
         </is>
       </c>
-      <c r="B173" s="71" t="n"/>
+      <c r="B173" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" ht="13.8" customHeight="1" s="45">
       <c r="A174" s="73" t="inlineStr">
@@ -2716,7 +2722,9 @@
           <t>Transaction level: Percentage of transactions including finance type</t>
         </is>
       </c>
-      <c r="B174" s="71" t="n"/>
+      <c r="B174" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" ht="13.8" customHeight="1" s="45">
       <c r="A175" s="73" t="inlineStr">
@@ -2724,7 +2732,7 @@
           <t>Transaction level: Finance type included in which transaction types?</t>
         </is>
       </c>
-      <c r="B175" s="71" t="n"/>
+      <c r="B175" s="71" t="inlineStr"/>
     </row>
     <row r="176" ht="13.8" customHeight="1" s="45">
       <c r="A176" s="73" t="inlineStr">
@@ -2732,7 +2740,11 @@
           <t>Which finance type is being used? .//default-finance-type/@code</t>
         </is>
       </c>
-      <c r="B176" s="71" t="n"/>
+      <c r="B176" s="71" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
     </row>
     <row r="177" ht="13.8" customHeight="1" s="45">
       <c r="A177" s="73" t="inlineStr">
@@ -2748,7 +2760,9 @@
           <t>Activity level: Number of activities including default flow type</t>
         </is>
       </c>
-      <c r="B178" s="71" t="n"/>
+      <c r="B178" s="71" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="179" ht="13.8" customHeight="1" s="45">
       <c r="A179" s="73" t="inlineStr">
@@ -2756,7 +2770,9 @@
           <t>Activity level: Percentage of activities including default flow type</t>
         </is>
       </c>
-      <c r="B179" s="72" t="n"/>
+      <c r="B179" s="72" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="180" ht="13.8" customHeight="1" s="45">
       <c r="A180" s="73" t="inlineStr">
@@ -2764,7 +2780,9 @@
           <t>Transaction level: Number of transactions including flow type</t>
         </is>
       </c>
-      <c r="B180" s="71" t="n"/>
+      <c r="B180" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" ht="13.8" customHeight="1" s="45">
       <c r="A181" s="73" t="inlineStr">
@@ -2772,7 +2790,9 @@
           <t>Transaction level: Percentage of transactions including flow type</t>
         </is>
       </c>
-      <c r="B181" s="71" t="n"/>
+      <c r="B181" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" ht="13.8" customHeight="1" s="45">
       <c r="A182" s="73" t="inlineStr">
@@ -2780,7 +2800,7 @@
           <t>Transaction level: Flow type included in which transaction types?</t>
         </is>
       </c>
-      <c r="B182" s="71" t="n"/>
+      <c r="B182" s="71" t="inlineStr"/>
     </row>
     <row r="183" ht="13.8" customHeight="1" s="45">
       <c r="A183" s="73" t="inlineStr">
@@ -2788,7 +2808,11 @@
           <t>Which flow type has been used? .//default-flow-type/@code</t>
         </is>
       </c>
-      <c r="B183" s="71" t="n"/>
+      <c r="B183" s="71" t="inlineStr">
+        <is>
+          <t>30, 10</t>
+        </is>
+      </c>
     </row>
     <row r="184" ht="13.8" customHeight="1" s="45">
       <c r="A184" s="57" t="n"/>
@@ -2827,7 +2851,9 @@
           <t>Activity level: Number of activities including default aid type</t>
         </is>
       </c>
-      <c r="B187" s="71" t="n"/>
+      <c r="B187" s="71" t="n">
+        <v>98</v>
+      </c>
     </row>
     <row r="188" ht="13.8" customHeight="1" s="45">
       <c r="A188" s="63" t="inlineStr">
@@ -2835,7 +2861,9 @@
           <t>Activity level: Percentage of activities including default aid type</t>
         </is>
       </c>
-      <c r="B188" s="72" t="n"/>
+      <c r="B188" s="72" t="n">
+        <v>98.98999999999999</v>
+      </c>
     </row>
     <row r="189" ht="13.8" customHeight="1" s="45">
       <c r="A189" s="63" t="inlineStr">
@@ -2843,7 +2871,9 @@
           <t>Transaction level: Number of transactions including aid type</t>
         </is>
       </c>
-      <c r="B189" s="71" t="n"/>
+      <c r="B189" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" ht="13.8" customHeight="1" s="45">
       <c r="A190" s="63" t="inlineStr">
@@ -2851,7 +2881,9 @@
           <t>Transaction level: Percentage of transactions including aid type</t>
         </is>
       </c>
-      <c r="B190" s="71" t="n"/>
+      <c r="B190" s="71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" ht="13.8" customHeight="1" s="45">
       <c r="A191" s="63" t="inlineStr">
@@ -2859,19 +2891,27 @@
           <t>Transaction level: Aid type included in which transaction types?</t>
         </is>
       </c>
-      <c r="B191" s="71" t="n"/>
-    </row>
-    <row r="192" ht="13.8" customHeight="1" s="45">
-      <c r="A192" s="63" t="inlineStr">
-        <is>
-          <t>Specify which aid type vocabularies have been used in addition to vocab 1? Have vocabs 2,3, 4 been used? (check activity and transaction level).</t>
-        </is>
-      </c>
-      <c r="B192" s="71" t="n"/>
-    </row>
-    <row r="193" ht="13.8" customHeight="1" s="45">
-      <c r="A193" s="55" t="n"/>
-      <c r="B193" s="64" t="n"/>
+      <c r="B191" s="71" t="inlineStr"/>
+    </row>
+    <row r="192" ht="14.15" customHeight="1" s="45">
+      <c r="A192" s="67" t="inlineStr">
+        <is>
+          <t>Which default aid type vocabularies are being used?</t>
+        </is>
+      </c>
+      <c r="B192" s="71" t="inlineStr">
+        <is>
+          <t>4, 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="193" ht="14.15" customHeight="1" s="45">
+      <c r="A193" s="67" t="inlineStr">
+        <is>
+          <t>Which aid type vocabularies are being used?</t>
+        </is>
+      </c>
+      <c r="B193" s="64" t="inlineStr"/>
     </row>
     <row r="194" ht="13.8" customHeight="1" s="45">
       <c r="I194" s="70" t="inlineStr">

</xml_diff>